<commit_message>
Inform Player, Waiting Server, Turn Start, Turn End, update doc
</commit_message>
<xml_diff>
--- a/message document.xlsx
+++ b/message document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Project\Magical-Wheel-Net\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D06C44E-66AD-4EE8-A6BB-55087B4DC2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C7D137-7CF7-4366-A55C-602503112005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
   <si>
     <t>Welcome</t>
   </si>
@@ -57,9 +57,6 @@
     <t>"Welcome to the server"</t>
   </si>
   <si>
-    <t>Game Start (max 2 player for now)</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>pkt id = 3</t>
   </si>
   <si>
-    <t>Turn</t>
-  </si>
-  <si>
     <t>pkt id = 4</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t>pkt id = 5</t>
   </si>
   <si>
-    <t>Correct</t>
-  </si>
-  <si>
     <t>Ntikhoa</t>
   </si>
   <si>
@@ -126,9 +117,6 @@
     <t>pkt id = 7</t>
   </si>
   <si>
-    <t>Incorrect</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -145,6 +133,21 @@
   </si>
   <si>
     <t>pkt id = 8</t>
+  </si>
+  <si>
+    <t>Inform Player (max 2 player for now)</t>
+  </si>
+  <si>
+    <t>timeout in seconds</t>
+  </si>
+  <si>
+    <t>Send Game Object (game start)</t>
+  </si>
+  <si>
+    <t>Turn Start</t>
+  </si>
+  <si>
+    <t>Turn End</t>
   </si>
 </sst>
 </file>
@@ -509,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J54"/>
+  <dimension ref="A2:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -532,7 +535,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -587,7 +590,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -600,346 +603,321 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1">
+        <v>10</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="1">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="1">
         <v>0</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>19</v>
+      <c r="D29" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="1">
+        <v>10</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="1">
         <v>0</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D34" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C46" s="1">
         <v>2</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C37" s="1">
+      <c r="D46" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="1">
         <v>0</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C43" s="1">
-        <v>0</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
-        <v>39</v>
+      <c r="D47" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C48" s="1">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C49" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C51" s="1">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C52" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C54" s="1">
-        <v>9</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rank player, disqualify, remove inform player
</commit_message>
<xml_diff>
--- a/message document.xlsx
+++ b/message document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Project\Magical-Wheel-Net\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C7D137-7CF7-4366-A55C-602503112005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B133F804-6E3F-48C7-AA5E-C60D519E8E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
   <si>
     <t>Welcome</t>
   </si>
@@ -111,9 +111,6 @@
     <t>score</t>
   </si>
   <si>
-    <t>current score</t>
-  </si>
-  <si>
     <t>pkt id = 7</t>
   </si>
   <si>
@@ -148,13 +145,19 @@
   </si>
   <si>
     <t>Turn End</t>
+  </si>
+  <si>
+    <t>turn</t>
+  </si>
+  <si>
+    <t>score get: 0, 1, 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +167,23 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -206,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -230,6 +250,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -512,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J52"/>
+  <dimension ref="A2:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -602,73 +628,84 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="A13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="10">
+        <v>2</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="1">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="10">
+        <v>1</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -706,12 +743,12 @@
         <v>10</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -741,182 +778,193 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="1">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C41" s="1">
-        <v>0</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" t="s">
-        <v>30</v>
+      <c r="A41" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="D43" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C46" s="1">
-        <v>2</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C47" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C49" s="1">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C50" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C53" s="1">
         <v>9</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add last guess and game end
</commit_message>
<xml_diff>
--- a/message document.xlsx
+++ b/message document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Project\Magical-Wheel-Net\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B133F804-6E3F-48C7-AA5E-C60D519E8E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A364FBD-5C05-4D66-899F-4717D9FF1C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
   <si>
     <t>Welcome</t>
   </si>
@@ -102,9 +102,6 @@
     <t>p*****</t>
   </si>
   <si>
-    <t>guest result</t>
-  </si>
-  <si>
     <t>client id</t>
   </si>
   <si>
@@ -151,6 +148,15 @@
   </si>
   <si>
     <t>score get: 0, 1, 5</t>
+  </si>
+  <si>
+    <t>guess result</t>
+  </si>
+  <si>
+    <t>guess word or char</t>
+  </si>
+  <si>
+    <t>p or python</t>
   </si>
 </sst>
 </file>
@@ -538,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J53"/>
+  <dimension ref="A2:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -629,7 +635,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -646,13 +652,13 @@
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="10">
         <v>2</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -697,7 +703,7 @@
         <v>10</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>10</v>
@@ -705,7 +711,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -743,12 +749,12 @@
         <v>10</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -786,12 +792,12 @@
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -807,7 +813,7 @@
         <v>0</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -829,7 +835,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -843,129 +849,140 @@
         <v>24</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" s="1">
-        <v>0</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" t="s">
-        <v>29</v>
+      <c r="A42" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="D44" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C47" s="1">
-        <v>2</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C48" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C50" s="1">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C51" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C53" s="1">
+        <v>10</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="1">
         <v>9</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>27</v>
+      <c r="D54" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>